<commit_message>
Replace Chlorobiaceae with Chlorobium
</commit_message>
<xml_diff>
--- a/06-figures_tables/Dataset_S4.xlsx
+++ b/06-figures_tables/Dataset_S4.xlsx
@@ -261,10 +261,10 @@
     <t>DLV002</t>
   </si>
   <si>
-    <t>Table S4b: Overview of the number of reads that could be aligned to the contigs of the Chlorobiaceae MAG of EMN001 for all dental calculus samples. The available short-read sequencing data were aligned against all contigs assembled from the sample EMN001 to avoid spurious alignments in the absence of any other reference genomes.</t>
-  </si>
-  <si>
-    <t># of reads against the Chlorobiaceae MAG</t>
+    <t>Table S4b: Overview of the number of reads that could be aligned to the contigs of the Chlorobium MAG of EMN001 for all dental calculus samples. The available short-read sequencing data were aligned against all contigs assembled from the sample EMN001 to avoid spurious alignments in the absence of any other reference genomes.</t>
+  </si>
+  <si>
+    <t># of reads against the Chlorobium MAG</t>
   </si>
   <si>
     <t>total # of reads</t>
@@ -273,7 +273,7 @@
     <t>% aligned</t>
   </si>
   <si>
-    <t>Table S4c: Overview of the snpAD genotyping results for the samples with strong evidence of Chlorobiaceae DNA. The number of sites to which at least a single read could be aligned and the sites genotypes are relative to the size of the EMN001 Chlorobiaceae MAG (1.88 Mb). Based on the number of genotyped sites, the fraction of sites with a homozygous genotype as the reference, with a heterozygous genotype, and a homozygous alternative genotype are reported. The remainder of the column lists the type of substitutions that were observed at sites with a homozygous alternative genotype.</t>
+    <t>Table S4c: Overview of the snpAD genotyping results for the samples with strong evidence of Chlorobium DNA. The number of sites to which at least a single read could be aligned and the sites genotypes are relative to the size of the EMN001 Chlorobium MAG (1.88 Mb). Based on the number of genotyped sites, the fraction of sites with a homozygous genotype as the reference, with a heterozygous genotype, and a homozygous alternative genotype are reported. The remainder of the column lists the type of substitutions that were observed at sites with a homozygous alternative genotype.</t>
   </si>
   <si>
     <t>sites with coverage &gt;= 1-fold</t>

</xml_diff>

<commit_message>
Add sample EMN001 to dataset S4b
</commit_message>
<xml_diff>
--- a/06-figures_tables/Dataset_S4.xlsx
+++ b/06-figures_tables/Dataset_S4.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
   <si>
     <t>ElSidron1</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>PLV001</t>
+  </si>
+  <si>
+    <t>EMN001</t>
   </si>
   <si>
     <t>RIG001</t>
@@ -799,7 +802,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -812,7 +815,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -820,13 +823,13 @@
         <v>13</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -848,13 +851,13 @@
         <v>19</v>
       </c>
       <c r="B5" s="2">
-        <v>6155371</v>
+        <v>6993330</v>
       </c>
       <c r="C5" s="2">
-        <v>176235843</v>
+        <v>189466499</v>
       </c>
       <c r="D5" s="5">
-        <v>3.49</v>
+        <v>3.69</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -862,13 +865,13 @@
         <v>20</v>
       </c>
       <c r="B6" s="2">
-        <v>2784287</v>
+        <v>6155371</v>
       </c>
       <c r="C6" s="2">
-        <v>125632680</v>
+        <v>176235843</v>
       </c>
       <c r="D6" s="5">
-        <v>2.22</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -876,13 +879,13 @@
         <v>21</v>
       </c>
       <c r="B7" s="2">
-        <v>2618352</v>
+        <v>2784287</v>
       </c>
       <c r="C7" s="2">
-        <v>17663236</v>
+        <v>125632680</v>
       </c>
       <c r="D7" s="5">
-        <v>14.82</v>
+        <v>2.22</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -890,13 +893,13 @@
         <v>22</v>
       </c>
       <c r="B8" s="2">
-        <v>932337</v>
+        <v>2618352</v>
       </c>
       <c r="C8" s="2">
-        <v>252714602</v>
+        <v>17663236</v>
       </c>
       <c r="D8" s="5">
-        <v>0.37</v>
+        <v>14.82</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -904,13 +907,13 @@
         <v>23</v>
       </c>
       <c r="B9" s="2">
-        <v>525993</v>
+        <v>932337</v>
       </c>
       <c r="C9" s="2">
-        <v>42008879</v>
+        <v>252714602</v>
       </c>
       <c r="D9" s="5">
-        <v>1.25</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -918,13 +921,13 @@
         <v>24</v>
       </c>
       <c r="B10" s="2">
-        <v>96605</v>
+        <v>525993</v>
       </c>
       <c r="C10" s="2">
-        <v>21690354</v>
+        <v>42008879</v>
       </c>
       <c r="D10" s="5">
-        <v>0.45</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -932,13 +935,13 @@
         <v>25</v>
       </c>
       <c r="B11" s="2">
-        <v>79390</v>
+        <v>96605</v>
       </c>
       <c r="C11" s="2">
-        <v>19093737</v>
+        <v>21690354</v>
       </c>
       <c r="D11" s="5">
-        <v>0.42</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -946,13 +949,13 @@
         <v>26</v>
       </c>
       <c r="B12" s="2">
-        <v>16457</v>
+        <v>79390</v>
       </c>
       <c r="C12" s="2">
-        <v>138768343</v>
+        <v>19093737</v>
       </c>
       <c r="D12" s="5">
-        <v>0.01</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -960,10 +963,10 @@
         <v>27</v>
       </c>
       <c r="B13" s="2">
-        <v>14074</v>
+        <v>16457</v>
       </c>
       <c r="C13" s="2">
-        <v>101440187</v>
+        <v>138768343</v>
       </c>
       <c r="D13" s="5">
         <v>0.01</v>
@@ -974,13 +977,13 @@
         <v>28</v>
       </c>
       <c r="B14" s="2">
-        <v>9876</v>
+        <v>14074</v>
       </c>
       <c r="C14" s="2">
-        <v>37162639</v>
+        <v>101440187</v>
       </c>
       <c r="D14" s="5">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -988,13 +991,13 @@
         <v>29</v>
       </c>
       <c r="B15" s="2">
-        <v>9018</v>
+        <v>9876</v>
       </c>
       <c r="C15" s="2">
-        <v>150151970</v>
+        <v>37162639</v>
       </c>
       <c r="D15" s="5">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1002,13 +1005,13 @@
         <v>30</v>
       </c>
       <c r="B16" s="2">
-        <v>8237</v>
+        <v>9018</v>
       </c>
       <c r="C16" s="2">
-        <v>231987190</v>
+        <v>150151970</v>
       </c>
       <c r="D16" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1016,13 +1019,13 @@
         <v>31</v>
       </c>
       <c r="B17" s="2">
-        <v>6970</v>
+        <v>8237</v>
       </c>
       <c r="C17" s="2">
-        <v>114228341</v>
+        <v>231987190</v>
       </c>
       <c r="D17" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1030,13 +1033,13 @@
         <v>32</v>
       </c>
       <c r="B18" s="2">
-        <v>6847</v>
+        <v>6970</v>
       </c>
       <c r="C18" s="2">
-        <v>142369309</v>
+        <v>114228341</v>
       </c>
       <c r="D18" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1044,10 +1047,10 @@
         <v>33</v>
       </c>
       <c r="B19" s="2">
-        <v>5397</v>
+        <v>6847</v>
       </c>
       <c r="C19" s="2">
-        <v>175558479</v>
+        <v>142369309</v>
       </c>
       <c r="D19" s="5">
         <v>0</v>
@@ -1058,38 +1061,38 @@
         <v>34</v>
       </c>
       <c r="B20" s="2">
-        <v>5045</v>
+        <v>5397</v>
       </c>
       <c r="C20" s="2">
-        <v>86929213</v>
+        <v>175558479</v>
       </c>
       <c r="D20" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2">
-        <v>4723</v>
+        <v>5045</v>
       </c>
       <c r="C21" s="2">
-        <v>95779863</v>
+        <v>86929213</v>
       </c>
       <c r="D21" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B22" s="2">
-        <v>3458</v>
+        <v>4723</v>
       </c>
       <c r="C22" s="2">
-        <v>71793405</v>
+        <v>95779863</v>
       </c>
       <c r="D22" s="5">
         <v>0</v>
@@ -1097,13 +1100,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="B23" s="2">
-        <v>3309</v>
+        <v>3458</v>
       </c>
       <c r="C23" s="2">
-        <v>88438101</v>
+        <v>71793405</v>
       </c>
       <c r="D23" s="5">
         <v>0</v>
@@ -1114,13 +1117,13 @@
         <v>36</v>
       </c>
       <c r="B24" s="2">
-        <v>2581</v>
+        <v>3309</v>
       </c>
       <c r="C24" s="2">
-        <v>42718432</v>
+        <v>88438101</v>
       </c>
       <c r="D24" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1128,10 +1131,10 @@
         <v>37</v>
       </c>
       <c r="B25" s="2">
-        <v>2557</v>
+        <v>2581</v>
       </c>
       <c r="C25" s="2">
-        <v>41407812</v>
+        <v>42718432</v>
       </c>
       <c r="D25" s="5">
         <v>0.01</v>
@@ -1142,13 +1145,13 @@
         <v>38</v>
       </c>
       <c r="B26" s="2">
-        <v>2554</v>
+        <v>2557</v>
       </c>
       <c r="C26" s="2">
-        <v>136507531</v>
+        <v>41407812</v>
       </c>
       <c r="D26" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1156,10 +1159,10 @@
         <v>39</v>
       </c>
       <c r="B27" s="2">
-        <v>2460</v>
+        <v>2554</v>
       </c>
       <c r="C27" s="2">
-        <v>104759552</v>
+        <v>136507531</v>
       </c>
       <c r="D27" s="5">
         <v>0</v>
@@ -1170,13 +1173,13 @@
         <v>40</v>
       </c>
       <c r="B28" s="2">
-        <v>2224</v>
+        <v>2460</v>
       </c>
       <c r="C28" s="2">
-        <v>30267110</v>
+        <v>104759552</v>
       </c>
       <c r="D28" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1184,13 +1187,13 @@
         <v>41</v>
       </c>
       <c r="B29" s="2">
-        <v>2100</v>
+        <v>2224</v>
       </c>
       <c r="C29" s="2">
-        <v>93467470</v>
+        <v>30267110</v>
       </c>
       <c r="D29" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1198,13 +1201,13 @@
         <v>42</v>
       </c>
       <c r="B30" s="2">
-        <v>1960</v>
+        <v>2100</v>
       </c>
       <c r="C30" s="2">
-        <v>32531519</v>
+        <v>93467470</v>
       </c>
       <c r="D30" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1212,13 +1215,13 @@
         <v>43</v>
       </c>
       <c r="B31" s="2">
-        <v>1764</v>
+        <v>1960</v>
       </c>
       <c r="C31" s="2">
-        <v>70138815</v>
+        <v>32531519</v>
       </c>
       <c r="D31" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1226,10 +1229,10 @@
         <v>44</v>
       </c>
       <c r="B32" s="2">
-        <v>1671</v>
+        <v>1764</v>
       </c>
       <c r="C32" s="2">
-        <v>67081666</v>
+        <v>70138815</v>
       </c>
       <c r="D32" s="5">
         <v>0</v>
@@ -1240,10 +1243,10 @@
         <v>45</v>
       </c>
       <c r="B33" s="2">
-        <v>1546</v>
+        <v>1671</v>
       </c>
       <c r="C33" s="2">
-        <v>100515321</v>
+        <v>67081666</v>
       </c>
       <c r="D33" s="5">
         <v>0</v>
@@ -1254,10 +1257,10 @@
         <v>46</v>
       </c>
       <c r="B34" s="2">
-        <v>1538</v>
+        <v>1546</v>
       </c>
       <c r="C34" s="2">
-        <v>103544825</v>
+        <v>100515321</v>
       </c>
       <c r="D34" s="5">
         <v>0</v>
@@ -1268,10 +1271,10 @@
         <v>47</v>
       </c>
       <c r="B35" s="2">
-        <v>1520</v>
+        <v>1538</v>
       </c>
       <c r="C35" s="2">
-        <v>103018785</v>
+        <v>103544825</v>
       </c>
       <c r="D35" s="5">
         <v>0</v>
@@ -1282,13 +1285,13 @@
         <v>48</v>
       </c>
       <c r="B36" s="2">
-        <v>1470</v>
+        <v>1520</v>
       </c>
       <c r="C36" s="2">
-        <v>22842128</v>
+        <v>103018785</v>
       </c>
       <c r="D36" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1296,10 +1299,10 @@
         <v>49</v>
       </c>
       <c r="B37" s="2">
-        <v>1457</v>
+        <v>1470</v>
       </c>
       <c r="C37" s="2">
-        <v>20678743</v>
+        <v>22842128</v>
       </c>
       <c r="D37" s="5">
         <v>0.01</v>
@@ -1310,13 +1313,13 @@
         <v>50</v>
       </c>
       <c r="B38" s="2">
-        <v>1417</v>
+        <v>1457</v>
       </c>
       <c r="C38" s="2">
-        <v>28804403</v>
+        <v>20678743</v>
       </c>
       <c r="D38" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1324,10 +1327,10 @@
         <v>51</v>
       </c>
       <c r="B39" s="2">
-        <v>1340</v>
+        <v>1417</v>
       </c>
       <c r="C39" s="2">
-        <v>97073118</v>
+        <v>28804403</v>
       </c>
       <c r="D39" s="5">
         <v>0</v>
@@ -1338,13 +1341,13 @@
         <v>52</v>
       </c>
       <c r="B40" s="2">
-        <v>1328</v>
+        <v>1340</v>
       </c>
       <c r="C40" s="2">
-        <v>25288494</v>
+        <v>97073118</v>
       </c>
       <c r="D40" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1352,13 +1355,13 @@
         <v>53</v>
       </c>
       <c r="B41" s="2">
-        <v>1257</v>
+        <v>1328</v>
       </c>
       <c r="C41" s="2">
-        <v>61253775</v>
+        <v>25288494</v>
       </c>
       <c r="D41" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1366,10 +1369,10 @@
         <v>54</v>
       </c>
       <c r="B42" s="2">
-        <v>1239</v>
+        <v>1257</v>
       </c>
       <c r="C42" s="2">
-        <v>33509960</v>
+        <v>61253775</v>
       </c>
       <c r="D42" s="5">
         <v>0</v>
@@ -1380,13 +1383,13 @@
         <v>55</v>
       </c>
       <c r="B43" s="2">
-        <v>1190</v>
+        <v>1239</v>
       </c>
       <c r="C43" s="2">
-        <v>20407221</v>
+        <v>33509960</v>
       </c>
       <c r="D43" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1394,13 +1397,13 @@
         <v>56</v>
       </c>
       <c r="B44" s="2">
-        <v>1160</v>
+        <v>1190</v>
       </c>
       <c r="C44" s="2">
-        <v>86648329</v>
+        <v>20407221</v>
       </c>
       <c r="D44" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1408,13 +1411,13 @@
         <v>57</v>
       </c>
       <c r="B45" s="2">
-        <v>1104</v>
+        <v>1160</v>
       </c>
       <c r="C45" s="2">
-        <v>18069068</v>
+        <v>86648329</v>
       </c>
       <c r="D45" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1422,13 +1425,13 @@
         <v>58</v>
       </c>
       <c r="B46" s="2">
-        <v>1017</v>
+        <v>1104</v>
       </c>
       <c r="C46" s="2">
-        <v>33789503</v>
+        <v>18069068</v>
       </c>
       <c r="D46" s="5">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1436,10 +1439,10 @@
         <v>59</v>
       </c>
       <c r="B47" s="2">
-        <v>936</v>
+        <v>1017</v>
       </c>
       <c r="C47" s="2">
-        <v>34114622</v>
+        <v>33789503</v>
       </c>
       <c r="D47" s="5">
         <v>0</v>
@@ -1450,10 +1453,10 @@
         <v>60</v>
       </c>
       <c r="B48" s="2">
-        <v>875</v>
+        <v>936</v>
       </c>
       <c r="C48" s="2">
-        <v>26733720</v>
+        <v>34114622</v>
       </c>
       <c r="D48" s="5">
         <v>0</v>
@@ -1464,10 +1467,10 @@
         <v>61</v>
       </c>
       <c r="B49" s="2">
-        <v>860</v>
+        <v>875</v>
       </c>
       <c r="C49" s="2">
-        <v>27271316</v>
+        <v>26733720</v>
       </c>
       <c r="D49" s="5">
         <v>0</v>
@@ -1478,10 +1481,10 @@
         <v>62</v>
       </c>
       <c r="B50" s="2">
-        <v>787</v>
+        <v>860</v>
       </c>
       <c r="C50" s="2">
-        <v>21989675</v>
+        <v>27271316</v>
       </c>
       <c r="D50" s="5">
         <v>0</v>
@@ -1492,10 +1495,10 @@
         <v>63</v>
       </c>
       <c r="B51" s="2">
-        <v>783</v>
+        <v>787</v>
       </c>
       <c r="C51" s="2">
-        <v>21118476</v>
+        <v>21989675</v>
       </c>
       <c r="D51" s="5">
         <v>0</v>
@@ -1506,10 +1509,10 @@
         <v>64</v>
       </c>
       <c r="B52" s="2">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="C52" s="2">
-        <v>85494014</v>
+        <v>21118476</v>
       </c>
       <c r="D52" s="5">
         <v>0</v>
@@ -1520,10 +1523,10 @@
         <v>65</v>
       </c>
       <c r="B53" s="2">
-        <v>766</v>
+        <v>780</v>
       </c>
       <c r="C53" s="2">
-        <v>20744859</v>
+        <v>85494014</v>
       </c>
       <c r="D53" s="5">
         <v>0</v>
@@ -1534,10 +1537,10 @@
         <v>66</v>
       </c>
       <c r="B54" s="2">
-        <v>752</v>
+        <v>766</v>
       </c>
       <c r="C54" s="2">
-        <v>15633770</v>
+        <v>20744859</v>
       </c>
       <c r="D54" s="5">
         <v>0</v>
@@ -1548,10 +1551,10 @@
         <v>67</v>
       </c>
       <c r="B55" s="2">
-        <v>743</v>
+        <v>752</v>
       </c>
       <c r="C55" s="2">
-        <v>51535506</v>
+        <v>15633770</v>
       </c>
       <c r="D55" s="5">
         <v>0</v>
@@ -1562,10 +1565,10 @@
         <v>68</v>
       </c>
       <c r="B56" s="2">
-        <v>706</v>
+        <v>743</v>
       </c>
       <c r="C56" s="2">
-        <v>19842423</v>
+        <v>51535506</v>
       </c>
       <c r="D56" s="5">
         <v>0</v>
@@ -1576,10 +1579,10 @@
         <v>69</v>
       </c>
       <c r="B57" s="2">
-        <v>693</v>
+        <v>706</v>
       </c>
       <c r="C57" s="2">
-        <v>65622476</v>
+        <v>19842423</v>
       </c>
       <c r="D57" s="5">
         <v>0</v>
@@ -1590,10 +1593,10 @@
         <v>70</v>
       </c>
       <c r="B58" s="2">
-        <v>576</v>
+        <v>693</v>
       </c>
       <c r="C58" s="2">
-        <v>19741755</v>
+        <v>65622476</v>
       </c>
       <c r="D58" s="5">
         <v>0</v>
@@ -1604,10 +1607,10 @@
         <v>71</v>
       </c>
       <c r="B59" s="2">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C59" s="2">
-        <v>31177646</v>
+        <v>19741755</v>
       </c>
       <c r="D59" s="5">
         <v>0</v>
@@ -1618,10 +1621,10 @@
         <v>72</v>
       </c>
       <c r="B60" s="2">
-        <v>438</v>
+        <v>574</v>
       </c>
       <c r="C60" s="2">
-        <v>17087811</v>
+        <v>31177646</v>
       </c>
       <c r="D60" s="5">
         <v>0</v>
@@ -1632,10 +1635,10 @@
         <v>73</v>
       </c>
       <c r="B61" s="2">
-        <v>344</v>
+        <v>438</v>
       </c>
       <c r="C61" s="2">
-        <v>37513542</v>
+        <v>17087811</v>
       </c>
       <c r="D61" s="5">
         <v>0</v>
@@ -1646,10 +1649,10 @@
         <v>74</v>
       </c>
       <c r="B62" s="2">
-        <v>277</v>
+        <v>344</v>
       </c>
       <c r="C62" s="2">
-        <v>21083888</v>
+        <v>37513542</v>
       </c>
       <c r="D62" s="5">
         <v>0</v>
@@ -1657,13 +1660,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="B63" s="2">
-        <v>259</v>
+        <v>277</v>
       </c>
       <c r="C63" s="2">
-        <v>7060628</v>
+        <v>21083888</v>
       </c>
       <c r="D63" s="5">
         <v>0</v>
@@ -1671,13 +1674,13 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B64" s="2">
-        <v>134</v>
+        <v>259</v>
       </c>
       <c r="C64" s="2">
-        <v>34298799</v>
+        <v>7060628</v>
       </c>
       <c r="D64" s="5">
         <v>0</v>
@@ -1685,13 +1688,13 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="B65" s="2">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="C65" s="2">
-        <v>24929320</v>
+        <v>34298799</v>
       </c>
       <c r="D65" s="5">
         <v>0</v>
@@ -1702,10 +1705,10 @@
         <v>76</v>
       </c>
       <c r="B66" s="2">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C66" s="2">
-        <v>6191314</v>
+        <v>24929320</v>
       </c>
       <c r="D66" s="5">
         <v>0</v>
@@ -1716,10 +1719,10 @@
         <v>77</v>
       </c>
       <c r="B67" s="2">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="C67" s="2">
-        <v>9122112</v>
+        <v>6191314</v>
       </c>
       <c r="D67" s="5">
         <v>0</v>
@@ -1730,10 +1733,10 @@
         <v>78</v>
       </c>
       <c r="B68" s="2">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C68" s="2">
-        <v>9122265</v>
+        <v>9122112</v>
       </c>
       <c r="D68" s="5">
         <v>0</v>
@@ -1744,10 +1747,10 @@
         <v>79</v>
       </c>
       <c r="B69" s="2">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C69" s="2">
-        <v>1578159</v>
+        <v>9122265</v>
       </c>
       <c r="D69" s="5">
         <v>0</v>
@@ -1758,12 +1761,26 @@
         <v>80</v>
       </c>
       <c r="B70" s="2">
+        <v>20</v>
+      </c>
+      <c r="C70" s="2">
+        <v>1578159</v>
+      </c>
+      <c r="D70" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B71" s="2">
         <v>6</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C71" s="2">
         <v>146302</v>
       </c>
-      <c r="D70" s="5">
+      <c r="D71" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1791,7 +1808,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1799,55 +1816,55 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -1908,7 +1925,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="7">
         <v>0.99783</v>
@@ -1964,7 +1981,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="7">
         <v>0.97458</v>
@@ -2020,7 +2037,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7">
         <v>0.97049</v>
@@ -2076,7 +2093,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="7">
         <v>0.96967</v>
@@ -2132,7 +2149,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7">
         <v>0.96216</v>
@@ -2188,7 +2205,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="7">
         <v>0.703</v>
@@ -2244,7 +2261,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7">
         <v>0.6449</v>

</xml_diff>

<commit_message>
Add additional columns for breadth and depth into Dataset S4
</commit_message>
<xml_diff>
--- a/06-figures_tables/Dataset_S4.xlsx
+++ b/06-figures_tables/Dataset_S4.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="108">
   <si>
     <t>ElSidron1</t>
   </si>
@@ -264,7 +264,7 @@
     <t>DLV002</t>
   </si>
   <si>
-    <t>Table S4b: Overview of the number of reads that could be aligned to the contigs of the Chlorobium MAG of EMN001 for all dental calculus samples. The available short-read sequencing data were aligned against all contigs assembled from the sample EMN001 to avoid spurious alignments in the absence of any other reference genomes.</t>
+    <t>Table S4b: Overview of the number of reads that could be aligned to the contigs of the Chlorobium MAG of EMN001 for all dental calculus samples. The available short-read sequencing data were aligned against all contigs assembled from the sample EMN001 to avoid spurious alignments in the absence of any other reference genomes. The number of contigs indicates to how many contigs reads could be aligned. For calculating the mean breadth, the mean depth, and the standard deviation of the depth, we first calculated the breadth and mean depth per contig and then summarised the data considering all contigs of the reference genome even when they were absent in the sample.</t>
   </si>
   <si>
     <t># of reads against the Chlorobium MAG</t>
@@ -274,6 +274,18 @@
   </si>
   <si>
     <t>% aligned</t>
+  </si>
+  <si>
+    <t># of contigs</t>
+  </si>
+  <si>
+    <t>mean breadth</t>
+  </si>
+  <si>
+    <t>mean depth</t>
+  </si>
+  <si>
+    <t>std depth</t>
   </si>
   <si>
     <t>Table S4c: Overview of the snpAD genotyping results for the samples with strong evidence of Chlorobium DNA. The number of sites to which at least a single read could be aligned and the sites genotypes are relative to the size of the EMN001 Chlorobium MAG (1.88 Mb). Based on the number of genotyped sites, the fraction of sites with a homozygous genotype as the reference, with a heterozygous genotype, and a homozygous alternative genotype are reported. The remainder of the column lists the type of substitutions that were observed at sites with a homozygous alternative genotype.</t>
@@ -802,23 +814,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="16.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:8">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
@@ -831,8 +848,20 @@
       <c r="D3" s="6" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -845,8 +874,20 @@
       <c r="D4" s="5">
         <v>11.56</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="2">
+        <v>21</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.997</v>
+      </c>
+      <c r="G4" s="5">
+        <v>314.314</v>
+      </c>
+      <c r="H4" s="5">
+        <v>102.755</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -859,8 +900,20 @@
       <c r="D5" s="5">
         <v>3.69</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="2">
+        <v>21</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="5">
+        <v>119.286</v>
+      </c>
+      <c r="H5" s="5">
+        <v>5.025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -873,8 +926,20 @@
       <c r="D6" s="5">
         <v>3.49</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="2">
+        <v>21</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.99</v>
+      </c>
+      <c r="G6" s="5">
+        <v>82.316</v>
+      </c>
+      <c r="H6" s="5">
+        <v>18.489</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -887,8 +952,20 @@
       <c r="D7" s="5">
         <v>2.22</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="2">
+        <v>21</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.973</v>
+      </c>
+      <c r="G7" s="5">
+        <v>51.262</v>
+      </c>
+      <c r="H7" s="5">
+        <v>9.266</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -901,8 +978,20 @@
       <c r="D8" s="5">
         <v>14.82</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="2">
+        <v>20</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.883</v>
+      </c>
+      <c r="G8" s="5">
+        <v>31.205</v>
+      </c>
+      <c r="H8" s="5">
+        <v>7.312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -915,8 +1004,20 @@
       <c r="D9" s="5">
         <v>0.37</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="2">
+        <v>21</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.962</v>
+      </c>
+      <c r="G9" s="5">
+        <v>21.301</v>
+      </c>
+      <c r="H9" s="5">
+        <v>4.181</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -929,8 +1030,20 @@
       <c r="D10" s="5">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" s="2">
+        <v>21</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="G10" s="5">
+        <v>11.015</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2.223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -943,8 +1056,20 @@
       <c r="D11" s="5">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" s="2">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.719</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2.016</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -957,8 +1082,20 @@
       <c r="D12" s="5">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="2">
+        <v>20</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.638</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1.704</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -971,8 +1108,20 @@
       <c r="D13" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="2">
+        <v>20</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.066</v>
+      </c>
+      <c r="G13" s="5">
+        <v>4.133</v>
+      </c>
+      <c r="H13" s="5">
+        <v>6.358</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -985,8 +1134,20 @@
       <c r="D14" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="2">
+        <v>21</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.215</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1.506</v>
+      </c>
+      <c r="H14" s="5">
+        <v>1.504</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -999,8 +1160,20 @@
       <c r="D15" s="5">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="2">
+        <v>21</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="G15" s="5">
+        <v>1.17</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.095</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -1013,8 +1186,20 @@
       <c r="D16" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" s="2">
+        <v>20</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.07199999999999999</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2.352</v>
+      </c>
+      <c r="H16" s="5">
+        <v>1.566</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1027,8 +1212,20 @@
       <c r="D17" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" s="2">
+        <v>21</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.059</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3.192</v>
+      </c>
+      <c r="H17" s="5">
+        <v>1.299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1041,8 +1238,20 @@
       <c r="D18" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" s="2">
+        <v>18</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.062</v>
+      </c>
+      <c r="G18" s="5">
+        <v>2.986</v>
+      </c>
+      <c r="H18" s="5">
+        <v>2.368</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1055,8 +1264,20 @@
       <c r="D19" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" s="2">
+        <v>17</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.011</v>
+      </c>
+      <c r="G19" s="5">
+        <v>5.329</v>
+      </c>
+      <c r="H19" s="5">
+        <v>6.616</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
@@ -1069,8 +1290,20 @@
       <c r="D20" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" s="2">
+        <v>20</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.022</v>
+      </c>
+      <c r="G20" s="5">
+        <v>3.584</v>
+      </c>
+      <c r="H20" s="5">
+        <v>2.426</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>35</v>
       </c>
@@ -1083,8 +1316,20 @@
       <c r="D21" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" s="2">
+        <v>19</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.026</v>
+      </c>
+      <c r="G21" s="5">
+        <v>3.403</v>
+      </c>
+      <c r="H21" s="5">
+        <v>3.595</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -1097,8 +1342,20 @@
       <c r="D22" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" s="2">
+        <v>17</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.049</v>
+      </c>
+      <c r="G22" s="5">
+        <v>2.623</v>
+      </c>
+      <c r="H22" s="5">
+        <v>5.385</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
@@ -1111,8 +1368,20 @@
       <c r="D23" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" s="2">
+        <v>21</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.057</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1.44</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -1125,8 +1394,20 @@
       <c r="D24" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" s="2">
+        <v>17</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G24" s="5">
+        <v>3.049</v>
+      </c>
+      <c r="H24" s="5">
+        <v>3.127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -1139,8 +1420,20 @@
       <c r="D25" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" s="2">
+        <v>19</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.049</v>
+      </c>
+      <c r="G25" s="5">
+        <v>2.01</v>
+      </c>
+      <c r="H25" s="5">
+        <v>1.016</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -1153,8 +1446,20 @@
       <c r="D26" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" s="2">
+        <v>18</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0.012</v>
+      </c>
+      <c r="G26" s="5">
+        <v>2.372</v>
+      </c>
+      <c r="H26" s="5">
+        <v>2.719</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -1167,8 +1472,20 @@
       <c r="D27" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" s="2">
+        <v>18</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.004</v>
+      </c>
+      <c r="G27" s="5">
+        <v>5.105</v>
+      </c>
+      <c r="H27" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -1181,8 +1498,20 @@
       <c r="D28" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" s="2">
+        <v>18</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0.003</v>
+      </c>
+      <c r="G28" s="5">
+        <v>4.493</v>
+      </c>
+      <c r="H28" s="5">
+        <v>6.793</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -1195,8 +1524,20 @@
       <c r="D29" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" s="2">
+        <v>19</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.032</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1.504</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0.854</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -1209,8 +1550,20 @@
       <c r="D30" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" s="2">
+        <v>16</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.003</v>
+      </c>
+      <c r="G30" s="5">
+        <v>4.056</v>
+      </c>
+      <c r="H30" s="5">
+        <v>6.867</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -1223,8 +1576,20 @@
       <c r="D31" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" s="2">
+        <v>18</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0.008</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1.857</v>
+      </c>
+      <c r="H31" s="5">
+        <v>1.426</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -1237,8 +1602,20 @@
       <c r="D32" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="2">
+        <v>15</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0.006</v>
+      </c>
+      <c r="G32" s="5">
+        <v>2.397</v>
+      </c>
+      <c r="H32" s="5">
+        <v>3.069</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -1251,8 +1628,20 @@
       <c r="D33" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" s="2">
+        <v>16</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0.045</v>
+      </c>
+      <c r="G33" s="5">
+        <v>2.775</v>
+      </c>
+      <c r="H33" s="5">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -1265,8 +1654,20 @@
       <c r="D34" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" s="2">
+        <v>17</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.006</v>
+      </c>
+      <c r="G34" s="5">
+        <v>2.512</v>
+      </c>
+      <c r="H34" s="5">
+        <v>2.194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -1279,8 +1680,20 @@
       <c r="D35" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="2">
+        <v>17</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.006</v>
+      </c>
+      <c r="G35" s="5">
+        <v>1.958</v>
+      </c>
+      <c r="H35" s="5">
+        <v>2.285</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -1293,8 +1706,20 @@
       <c r="D36" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" s="2">
+        <v>17</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0.008</v>
+      </c>
+      <c r="G36" s="5">
+        <v>2.551</v>
+      </c>
+      <c r="H36" s="5">
+        <v>1.871</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>49</v>
       </c>
@@ -1307,8 +1732,20 @@
       <c r="D37" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" s="2">
+        <v>17</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="G37" s="5">
+        <v>1.338</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0.904</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>50</v>
       </c>
@@ -1321,8 +1758,20 @@
       <c r="D38" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" s="2">
+        <v>16</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0.006</v>
+      </c>
+      <c r="G38" s="5">
+        <v>1.188</v>
+      </c>
+      <c r="H38" s="5">
+        <v>1.203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>51</v>
       </c>
@@ -1335,8 +1784,20 @@
       <c r="D39" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" s="2">
+        <v>18</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.006</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1.148</v>
+      </c>
+      <c r="H39" s="5">
+        <v>1.019</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>52</v>
       </c>
@@ -1349,8 +1810,20 @@
       <c r="D40" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
+      <c r="E40" s="2">
+        <v>18</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0.039</v>
+      </c>
+      <c r="G40" s="5">
+        <v>3.047</v>
+      </c>
+      <c r="H40" s="5">
+        <v>3.769</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>53</v>
       </c>
@@ -1363,8 +1836,20 @@
       <c r="D41" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E41" s="2">
+        <v>16</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0.047</v>
+      </c>
+      <c r="G41" s="5">
+        <v>1.723</v>
+      </c>
+      <c r="H41" s="5">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>54</v>
       </c>
@@ -1377,8 +1862,20 @@
       <c r="D42" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" s="2">
+        <v>18</v>
+      </c>
+      <c r="F42" s="5">
+        <v>0.003</v>
+      </c>
+      <c r="G42" s="5">
+        <v>3.497</v>
+      </c>
+      <c r="H42" s="5">
+        <v>5.911</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>55</v>
       </c>
@@ -1391,8 +1888,20 @@
       <c r="D43" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" s="2">
+        <v>19</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0.008</v>
+      </c>
+      <c r="G43" s="5">
+        <v>1.341</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0.653</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>56</v>
       </c>
@@ -1405,8 +1914,20 @@
       <c r="D44" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" s="2">
+        <v>19</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0.027</v>
+      </c>
+      <c r="G44" s="5">
+        <v>1.442</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0.644</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>57</v>
       </c>
@@ -1419,8 +1940,20 @@
       <c r="D45" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" s="2">
+        <v>18</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0.006</v>
+      </c>
+      <c r="G45" s="5">
+        <v>2.446</v>
+      </c>
+      <c r="H45" s="5">
+        <v>2.933</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>58</v>
       </c>
@@ -1433,8 +1966,20 @@
       <c r="D46" s="5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" s="2">
+        <v>16</v>
+      </c>
+      <c r="F46" s="5">
+        <v>0.005</v>
+      </c>
+      <c r="G46" s="5">
+        <v>1.007</v>
+      </c>
+      <c r="H46" s="5">
+        <v>0.886</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>59</v>
       </c>
@@ -1447,8 +1992,20 @@
       <c r="D47" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" s="2">
+        <v>19</v>
+      </c>
+      <c r="F47" s="5">
+        <v>0.005</v>
+      </c>
+      <c r="G47" s="5">
+        <v>1.957</v>
+      </c>
+      <c r="H47" s="5">
+        <v>1.462</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>60</v>
       </c>
@@ -1461,8 +2018,20 @@
       <c r="D48" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48" s="2">
+        <v>17</v>
+      </c>
+      <c r="F48" s="5">
+        <v>0.036</v>
+      </c>
+      <c r="G48" s="5">
+        <v>1.582</v>
+      </c>
+      <c r="H48" s="5">
+        <v>1.088</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>61</v>
       </c>
@@ -1475,8 +2044,20 @@
       <c r="D49" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" s="2">
+        <v>15</v>
+      </c>
+      <c r="F49" s="5">
+        <v>0.004</v>
+      </c>
+      <c r="G49" s="5">
+        <v>1.044</v>
+      </c>
+      <c r="H49" s="5">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
@@ -1489,8 +2070,20 @@
       <c r="D50" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
+      <c r="E50" s="2">
+        <v>18</v>
+      </c>
+      <c r="F50" s="5">
+        <v>0.022</v>
+      </c>
+      <c r="G50" s="5">
+        <v>1.332</v>
+      </c>
+      <c r="H50" s="5">
+        <v>0.712</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>63</v>
       </c>
@@ -1503,8 +2096,20 @@
       <c r="D51" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E51" s="2">
+        <v>19</v>
+      </c>
+      <c r="F51" s="5">
+        <v>0.011</v>
+      </c>
+      <c r="G51" s="5">
+        <v>1.297</v>
+      </c>
+      <c r="H51" s="5">
+        <v>0.521</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>64</v>
       </c>
@@ -1517,8 +2122,20 @@
       <c r="D52" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" s="2">
+        <v>16</v>
+      </c>
+      <c r="F52" s="5">
+        <v>0.004</v>
+      </c>
+      <c r="G52" s="5">
+        <v>1.119</v>
+      </c>
+      <c r="H52" s="5">
+        <v>0.771</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>65</v>
       </c>
@@ -1531,8 +2148,20 @@
       <c r="D53" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" s="2">
+        <v>17</v>
+      </c>
+      <c r="F53" s="5">
+        <v>0.003</v>
+      </c>
+      <c r="G53" s="5">
+        <v>1.969</v>
+      </c>
+      <c r="H53" s="5">
+        <v>1.951</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>66</v>
       </c>
@@ -1545,8 +2174,20 @@
       <c r="D54" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54" s="2">
+        <v>17</v>
+      </c>
+      <c r="F54" s="5">
+        <v>0.006</v>
+      </c>
+      <c r="G54" s="5">
+        <v>0.999</v>
+      </c>
+      <c r="H54" s="5">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
         <v>67</v>
       </c>
@@ -1559,8 +2200,20 @@
       <c r="D55" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55" s="2">
+        <v>16</v>
+      </c>
+      <c r="F55" s="5">
+        <v>0.013</v>
+      </c>
+      <c r="G55" s="5">
+        <v>1.03</v>
+      </c>
+      <c r="H55" s="5">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
         <v>68</v>
       </c>
@@ -1573,8 +2226,20 @@
       <c r="D56" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56" s="2">
+        <v>18</v>
+      </c>
+      <c r="F56" s="5">
+        <v>0.003</v>
+      </c>
+      <c r="G56" s="5">
+        <v>2.206</v>
+      </c>
+      <c r="H56" s="5">
+        <v>1.862</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>69</v>
       </c>
@@ -1587,8 +2252,20 @@
       <c r="D57" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" s="2">
+        <v>18</v>
+      </c>
+      <c r="F57" s="5">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="G57" s="5">
+        <v>1.259</v>
+      </c>
+      <c r="H57" s="5">
+        <v>0.645</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
         <v>70</v>
       </c>
@@ -1601,8 +2278,20 @@
       <c r="D58" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58" s="2">
+        <v>18</v>
+      </c>
+      <c r="F58" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="G58" s="5">
+        <v>1.712</v>
+      </c>
+      <c r="H58" s="5">
+        <v>1.546</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
         <v>71</v>
       </c>
@@ -1615,8 +2304,20 @@
       <c r="D59" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59" s="2">
+        <v>16</v>
+      </c>
+      <c r="F59" s="5">
+        <v>0.037</v>
+      </c>
+      <c r="G59" s="5">
+        <v>1.096</v>
+      </c>
+      <c r="H59" s="5">
+        <v>0.734</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
         <v>72</v>
       </c>
@@ -1629,8 +2330,20 @@
       <c r="D60" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
+      <c r="E60" s="2">
+        <v>17</v>
+      </c>
+      <c r="F60" s="5">
+        <v>0.019</v>
+      </c>
+      <c r="G60" s="5">
+        <v>1.388</v>
+      </c>
+      <c r="H60" s="5">
+        <v>0.9429999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
         <v>73</v>
       </c>
@@ -1643,8 +2356,20 @@
       <c r="D61" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61" s="2">
+        <v>16</v>
+      </c>
+      <c r="F61" s="5">
+        <v>0.026</v>
+      </c>
+      <c r="G61" s="5">
+        <v>1.133</v>
+      </c>
+      <c r="H61" s="5">
+        <v>0.959</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>74</v>
       </c>
@@ -1657,8 +2382,20 @@
       <c r="D62" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62" s="2">
+        <v>13</v>
+      </c>
+      <c r="F62" s="5">
+        <v>0.003</v>
+      </c>
+      <c r="G62" s="5">
+        <v>0.9429999999999999</v>
+      </c>
+      <c r="H62" s="5">
+        <v>0.831</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>75</v>
       </c>
@@ -1671,8 +2408,20 @@
       <c r="D63" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63" s="2">
+        <v>16</v>
+      </c>
+      <c r="F63" s="5">
+        <v>0.002</v>
+      </c>
+      <c r="G63" s="5">
+        <v>1.103</v>
+      </c>
+      <c r="H63" s="5">
+        <v>0.748</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
         <v>3</v>
       </c>
@@ -1685,8 +2434,20 @@
       <c r="D64" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64" s="2">
+        <v>11</v>
+      </c>
+      <c r="F64" s="5">
+        <v>0.001</v>
+      </c>
+      <c r="G64" s="5">
+        <v>1.917</v>
+      </c>
+      <c r="H64" s="5">
+        <v>2.433</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
         <v>2</v>
       </c>
@@ -1699,8 +2460,20 @@
       <c r="D65" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65" s="2">
+        <v>14</v>
+      </c>
+      <c r="F65" s="5">
+        <v>0.001</v>
+      </c>
+      <c r="G65" s="5">
+        <v>0.982</v>
+      </c>
+      <c r="H65" s="5">
+        <v>0.911</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
         <v>76</v>
       </c>
@@ -1713,8 +2486,20 @@
       <c r="D66" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66" s="2">
+        <v>11</v>
+      </c>
+      <c r="F66" s="5">
+        <v>0</v>
+      </c>
+      <c r="G66" s="5">
+        <v>0.5620000000000001</v>
+      </c>
+      <c r="H66" s="5">
+        <v>0.992</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
         <v>77</v>
       </c>
@@ -1727,8 +2512,20 @@
       <c r="D67" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67" s="2">
+        <v>11</v>
+      </c>
+      <c r="F67" s="5">
+        <v>0.001</v>
+      </c>
+      <c r="G67" s="5">
+        <v>0.595</v>
+      </c>
+      <c r="H67" s="5">
+        <v>0.599</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
         <v>78</v>
       </c>
@@ -1741,8 +2538,20 @@
       <c r="D68" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68" s="2">
+        <v>8</v>
+      </c>
+      <c r="F68" s="5">
+        <v>0</v>
+      </c>
+      <c r="G68" s="5">
+        <v>0.393</v>
+      </c>
+      <c r="H68" s="5">
+        <v>0.515</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
         <v>79</v>
       </c>
@@ -1755,8 +2564,20 @@
       <c r="D69" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69" s="2">
+        <v>9</v>
+      </c>
+      <c r="F69" s="5">
+        <v>0</v>
+      </c>
+      <c r="G69" s="5">
+        <v>0.485</v>
+      </c>
+      <c r="H69" s="5">
+        <v>0.626</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
         <v>80</v>
       </c>
@@ -1769,8 +2590,20 @@
       <c r="D70" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:4">
+      <c r="E70" s="2">
+        <v>8</v>
+      </c>
+      <c r="F70" s="5">
+        <v>0</v>
+      </c>
+      <c r="G70" s="5">
+        <v>0.235</v>
+      </c>
+      <c r="H70" s="5">
+        <v>0.431</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
         <v>81</v>
       </c>
@@ -1782,6 +2615,18 @@
       </c>
       <c r="D71" s="5">
         <v>0</v>
+      </c>
+      <c r="E71" s="2">
+        <v>3</v>
+      </c>
+      <c r="F71" s="5">
+        <v>0</v>
+      </c>
+      <c r="G71" s="5">
+        <v>0.143</v>
+      </c>
+      <c r="H71" s="5">
+        <v>0.359</v>
       </c>
     </row>
   </sheetData>
@@ -1808,7 +2653,7 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1816,55 +2661,55 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:18">

</xml_diff>